<commit_message>
DEV - Goal is done
</commit_message>
<xml_diff>
--- a/docs/development plan.xlsx
+++ b/docs/development plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
   <si>
     <t>Search</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t>David Löffler, Miroslav Rudišin</t>
+  </si>
+  <si>
+    <t>Yevgeniya Chekh</t>
+  </si>
+  <si>
+    <t>Miroslav Rudišin, Kryštof Sýkora</t>
   </si>
 </sst>
 </file>
@@ -549,6 +555,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -582,11 +590,9 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -893,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B24" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+    <sheetView tabSelected="1" topLeftCell="B26" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,37 +919,37 @@
       <c r="C6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="29">
         <v>5</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="29">
         <v>6</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="29">
         <v>7</v>
       </c>
-      <c r="G6" s="27">
+      <c r="G6" s="29">
         <v>8</v>
       </c>
-      <c r="H6" s="27">
+      <c r="H6" s="29">
         <v>9</v>
       </c>
-      <c r="I6" s="27">
+      <c r="I6" s="29">
         <v>10</v>
       </c>
-      <c r="J6" s="27">
+      <c r="J6" s="29">
         <v>11</v>
       </c>
-      <c r="K6" s="27">
+      <c r="K6" s="29">
         <v>12</v>
       </c>
-      <c r="L6" s="27">
+      <c r="L6" s="29">
         <v>13</v>
       </c>
-      <c r="M6" s="22">
+      <c r="M6" s="24">
         <v>14</v>
       </c>
-      <c r="N6" s="22" t="s">
+      <c r="N6" s="24" t="s">
         <v>21</v>
       </c>
     </row>
@@ -951,17 +957,17 @@
       <c r="C7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C8" s="5" t="s">
@@ -1184,34 +1190,34 @@
       </c>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="30"/>
-      <c r="M21" s="31"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="33"/>
     </row>
     <row r="22" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
-      <c r="M22" s="26"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="28"/>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
@@ -1223,37 +1229,37 @@
       <c r="C27" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="27">
+      <c r="D27" s="29">
         <v>5</v>
       </c>
-      <c r="E27" s="27">
+      <c r="E27" s="29">
         <v>6</v>
       </c>
-      <c r="F27" s="27">
+      <c r="F27" s="29">
         <v>7</v>
       </c>
-      <c r="G27" s="27">
+      <c r="G27" s="29">
         <v>8</v>
       </c>
-      <c r="H27" s="27">
+      <c r="H27" s="29">
         <v>9</v>
       </c>
-      <c r="I27" s="27">
+      <c r="I27" s="29">
         <v>10</v>
       </c>
-      <c r="J27" s="27">
+      <c r="J27" s="29">
         <v>11</v>
       </c>
-      <c r="K27" s="27">
+      <c r="K27" s="29">
         <v>12</v>
       </c>
-      <c r="L27" s="27">
+      <c r="L27" s="29">
         <v>13</v>
       </c>
-      <c r="M27" s="22">
+      <c r="M27" s="24">
         <v>14</v>
       </c>
-      <c r="N27" s="22" t="s">
+      <c r="N27" s="24" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1261,24 +1267,24 @@
       <c r="C28" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="23"/>
-      <c r="N28" s="23"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
+      <c r="K28" s="30"/>
+      <c r="L28" s="30"/>
+      <c r="M28" s="25"/>
+      <c r="N28" s="25"/>
     </row>
     <row r="29" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C29" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
@@ -1323,18 +1329,20 @@
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="3"/>
-      <c r="N31" s="21"/>
+      <c r="N31" s="21" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="32" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C32" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D32" s="32" t="s">
+      <c r="D32" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="35"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="23"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -1427,7 +1435,9 @@
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="3"/>
-      <c r="N37" s="21"/>
+      <c r="N37" s="21" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="38" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C38" s="2" t="s">
@@ -1498,34 +1508,34 @@
       </c>
     </row>
     <row r="42" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C42" s="29" t="s">
+      <c r="C42" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="D42" s="30"/>
-      <c r="E42" s="30"/>
-      <c r="F42" s="30"/>
-      <c r="G42" s="30"/>
-      <c r="H42" s="30"/>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
-      <c r="K42" s="30"/>
-      <c r="L42" s="30"/>
-      <c r="M42" s="31"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="32"/>
+      <c r="G42" s="32"/>
+      <c r="H42" s="32"/>
+      <c r="I42" s="32"/>
+      <c r="J42" s="32"/>
+      <c r="K42" s="32"/>
+      <c r="L42" s="32"/>
+      <c r="M42" s="33"/>
     </row>
     <row r="43" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C43" s="24" t="s">
+      <c r="C43" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="25"/>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
-      <c r="K43" s="25"/>
-      <c r="L43" s="25"/>
-      <c r="M43" s="26"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
+      <c r="K43" s="27"/>
+      <c r="L43" s="27"/>
+      <c r="M43" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="27">

</xml_diff>